<commit_message>
Inserted figures, updated Excel sheets
</commit_message>
<xml_diff>
--- a/Benchmark_GPUPI.xlsx
+++ b/Benchmark_GPUPI.xlsx
@@ -111,7 +111,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-AT"/>
-              <a:t>100 Millionen Nachkommastellen von PI</a:t>
+              <a:t>GPUPI - 100 Millionen Nachkommastellen von PI</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -399,11 +399,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54634496"/>
-        <c:axId val="86401600"/>
+        <c:axId val="120162304"/>
+        <c:axId val="88435520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54634496"/>
+        <c:axId val="120162304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +431,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86401600"/>
+        <c:crossAx val="88435520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -439,7 +439,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86401600"/>
+        <c:axId val="88435520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,7 +469,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54634496"/>
+        <c:crossAx val="120162304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -525,6 +525,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="de-AT" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>GPUPI - </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="de-AT"/>
               <a:t>1 Milliarde Nachkommastellen von PI</a:t>
             </a:r>
@@ -882,11 +888,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="129923584"/>
-        <c:axId val="86427328"/>
+        <c:axId val="120233472"/>
+        <c:axId val="88437824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="129923584"/>
+        <c:axId val="120233472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -964,7 +970,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86427328"/>
+        <c:crossAx val="88437824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -972,7 +978,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86427328"/>
+        <c:axId val="88437824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1065,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="129923584"/>
+        <c:crossAx val="120233472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1164,6 +1170,12 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="de-AT" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>GPUPI - </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="de-AT"/>
               <a:t>2 Milliarden Nachkommastellen von PI</a:t>
             </a:r>
@@ -1453,11 +1465,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54840320"/>
-        <c:axId val="86820544"/>
+        <c:axId val="94352896"/>
+        <c:axId val="88440128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54840320"/>
+        <c:axId val="94352896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1497,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86820544"/>
+        <c:crossAx val="88440128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1493,7 +1505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86820544"/>
+        <c:axId val="88440128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,7 +1535,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54840320"/>
+        <c:crossAx val="94352896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2461,7 +2473,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>